<commit_message>
fix: change excel template file
</commit_message>
<xml_diff>
--- a/public/excel/request_orders_template.xlsx
+++ b/public/excel/request_orders_template.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w.jaitnipat\Developer\aes-project\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L.kritsada\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="4956"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="4950"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DropdownList" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>หัวตารางแจ้งงาน</t>
   </si>
@@ -71,18 +72,12 @@
     <t>ไร่บริษัท</t>
   </si>
   <si>
-    <t>099-999-9999</t>
-  </si>
-  <si>
     <t>RDC0</t>
   </si>
   <si>
     <t>น้ำปลีก</t>
   </si>
   <si>
-    <t>POLYGON((102.25297562 16.22933296,102.24774915 16.23109708,102.24829965 16.23239083,102.24840038 16.23253653,102.24845718 16.23267447,102.2486908 16.23316208,102.24878102 16.23347415,102.24982015 16.23314193,102.25049242 16.23280154,102.25098552 16.2325321,102.25149342 16.23227249,102.25183211 16.23207591,102.25176576 16.23188483,102.25205707 16.23173843,102.2531239 16.23123115,102.2536032 16.23100074,102.25337511 16.23042657,102.25297562 16.22933296))</t>
-  </si>
-  <si>
     <t>ปรับพื้นที่ / ดันกอง+ไถกลบเศษซาก+ไถพรวน 1</t>
   </si>
   <si>
@@ -92,14 +87,59 @@
     <t>เมษายน</t>
   </si>
   <si>
-    <t>นายสิริ วิโรธ</t>
+    <t>POLYGON((102.25297562 16.22933296,102.24774915 16.23109708))</t>
+  </si>
+  <si>
+    <t>(ตัวอย่าง)</t>
+  </si>
+  <si>
+    <t>0XX-XXX-XXXX</t>
+  </si>
+  <si>
+    <t>มกราคม</t>
+  </si>
+  <si>
+    <t>กุมภาพันธ์</t>
+  </si>
+  <si>
+    <t>มีนาคม</t>
+  </si>
+  <si>
+    <t>พฤษภาคม</t>
+  </si>
+  <si>
+    <t>มิถุนายน</t>
+  </si>
+  <si>
+    <t>กรกฎาคม</t>
+  </si>
+  <si>
+    <t>สิงหาคม</t>
+  </si>
+  <si>
+    <t>กันยายน</t>
+  </si>
+  <si>
+    <t>ตุลาคม</t>
+  </si>
+  <si>
+    <t>พฤศจิกายน</t>
+  </si>
+  <si>
+    <t>ธันวาคม</t>
+  </si>
+  <si>
+    <t>ชาวไร่มิตรผล</t>
+  </si>
+  <si>
+    <t>ชาวไร่ภายนอก</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,16 +148,48 @@
       <charset val="222"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="TH SarabunPSK"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="TH SarabunPSK"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="TH SarabunPSK"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -125,14 +197,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -414,207 +530,403 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.8984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.69921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37.19921875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="65.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.8984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.8984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="12.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="2" customWidth="1"/>
+    <col min="7" max="8" width="14.25" style="2" customWidth="1"/>
+    <col min="9" max="9" width="55.5" style="2" customWidth="1"/>
+    <col min="10" max="10" width="32.375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="48.5" style="2" customWidth="1"/>
+    <col min="12" max="13" width="9.625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="12.5" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="9.125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="8">
+        <v>110302</v>
+      </c>
+      <c r="E2" s="8">
+        <v>110302</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="8">
+        <v>25</v>
+      </c>
+      <c r="H2" s="8">
+        <v>110302106</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="8">
+        <v>2568</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="N2LwYQnpmZOKMGwL23c+YlQ+DDi8NhCWMSrltO3dOLB6PzCvHFX1U4O0m9zNDs1fwupltykGmzCag8YRS/gwFQ==" saltValue="09rJKPUzTrayklKRIYpOaw==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <protectedRanges>
+    <protectedRange algorithmName="SHA-512" hashValue="5GdnB8tTru9JA2O74AjBU+R/ItLoMktBIoCoPkQyHJrYgTc7bvPFBp/1Dru2jk9gHsm6XdxPG5DBYZKkUwiYmw==" saltValue="bF8GF9kdjmly4KvsuqEbAg==" spinCount="100000" sqref="A1:N2" name="Range1"/>
+  </protectedRanges>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>DropdownList!$B$2:$B$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>L2:L1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>DropdownList!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>A3:A1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="9" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1">
-        <v>110302</v>
-      </c>
-      <c r="E2" s="1">
-        <v>110302</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="1">
-        <v>110302106</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="1" t="s">
+    </row>
+    <row r="5" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="1">
-        <v>2568</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="1">
-        <v>110302</v>
-      </c>
-      <c r="E3" s="1">
-        <v>110302</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1">
-        <v>25</v>
-      </c>
-      <c r="H3" s="1">
-        <v>110302106</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="1">
-        <v>2568</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="1">
-        <v>110302</v>
-      </c>
-      <c r="E4" s="1">
-        <v>110302</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="1">
-        <v>25</v>
-      </c>
-      <c r="H4" s="1">
-        <v>110302106</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" s="1">
-        <v>2568</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>22</v>
+    </row>
+    <row r="6" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="rEmDEZvuKE5gphMWXAey6LzgrksjY3UBditRvLj0TFwr3qLwvDmdMskhLAhMTKO5UagJfWynriXKGw9x36624Q==" saltValue="dPZH1hUDzKKVV1OvElbdlQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add date input fields and improve UI components; implement TODOs for better functionality
</commit_message>
<xml_diff>
--- a/public/excel/request_orders_template.xlsx
+++ b/public/excel/request_orders_template.xlsx
@@ -158,7 +158,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +191,12 @@
       <color rgb="FF000000"/>
       <name val="JetBrainsMono NF"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="TH SarabunPSK"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -245,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -253,40 +259,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -596,7 +603,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -609,53 +616,54 @@
     <col min="8" max="8" width="55.625" style="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="32.375" style="13" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="48.625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.625" style="14" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
@@ -696,7 +704,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="12"/>
@@ -707,11 +715,10 @@
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
-      <c r="K3" s="3"/>
       <c r="L3" s="12"/>
       <c r="M3" s="11"/>
     </row>
-    <row r="4" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="12"/>
@@ -722,11 +729,10 @@
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
-      <c r="K4" s="3"/>
       <c r="L4" s="12"/>
       <c r="M4" s="11"/>
     </row>
-    <row r="5" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
@@ -737,11 +743,10 @@
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
-      <c r="K5" s="3"/>
       <c r="L5" s="12"/>
       <c r="M5" s="11"/>
     </row>
-    <row r="6" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
@@ -752,11 +757,10 @@
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
-      <c r="K6" s="3"/>
       <c r="L6" s="12"/>
       <c r="M6" s="11"/>
     </row>
-    <row r="7" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
@@ -767,11 +771,10 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
-      <c r="K7" s="3"/>
       <c r="L7" s="12"/>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
@@ -782,11 +785,10 @@
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
-      <c r="K8" s="3"/>
       <c r="L8" s="12"/>
       <c r="M8" s="11"/>
     </row>
-    <row r="9" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="12"/>
@@ -797,11 +799,10 @@
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
-      <c r="K9" s="3"/>
       <c r="L9" s="12"/>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="12"/>
@@ -812,11 +813,10 @@
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
-      <c r="K10" s="3"/>
       <c r="L10" s="12"/>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="12"/>
@@ -827,11 +827,10 @@
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
-      <c r="K11" s="3"/>
       <c r="L11" s="12"/>
       <c r="M11" s="11"/>
     </row>
-    <row r="12" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="12"/>
@@ -842,11 +841,10 @@
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
-      <c r="K12" s="3"/>
       <c r="L12" s="12"/>
       <c r="M12" s="11"/>
     </row>
-    <row r="13" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="12"/>
@@ -857,12 +855,12 @@
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
-      <c r="K13" s="3"/>
       <c r="L13" s="12"/>
       <c r="M13" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -897,7 +895,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.25" style="5" customWidth="1"/>
+    <col min="1" max="1" width="12.25" style="3" customWidth="1"/>
     <col min="2" max="2" width="15.75" customWidth="1"/>
   </cols>
   <sheetData>
@@ -913,7 +911,7 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="4" t="s">
         <v>26</v>
       </c>
     </row>
@@ -921,7 +919,7 @@
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -929,7 +927,7 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -937,7 +935,7 @@
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="4" t="s">
         <v>34</v>
       </c>
     </row>
@@ -945,7 +943,7 @@
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -953,7 +951,7 @@
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -961,7 +959,7 @@
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -969,7 +967,7 @@
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -977,7 +975,7 @@
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -985,7 +983,7 @@
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -993,7 +991,7 @@
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="4" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1001,12 +999,12 @@
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="4" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>